<commit_message>
jar file and postman collection added
</commit_message>
<xml_diff>
--- a/timetable_1.xlsx
+++ b/timetable_1.xlsx
@@ -35,19 +35,16 @@
     <t/>
   </si>
   <si>
+    <t>Music</t>
+  </si>
+  <si>
     <t>Math</t>
   </si>
   <si>
-    <t>Polish</t>
+    <t>Physics</t>
   </si>
   <si>
-    <t>Religion</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Physics</t>
+    <t>Polish</t>
   </si>
   <si>
     <t>PE</t>
@@ -56,7 +53,10 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>Music</t>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Religion</t>
   </si>
   <si>
     <t>IB</t>
@@ -231,7 +231,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>6</v>
@@ -242,13 +242,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>6</v>
@@ -256,13 +256,13 @@
     </row>
     <row r="5">
       <c r="B5" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>8</v>
@@ -273,36 +273,36 @@
     </row>
     <row r="6">
       <c r="B6" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>12</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -310,16 +310,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -327,16 +327,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -344,16 +344,16 @@
         <v>6</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -364,7 +364,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>6</v>
@@ -415,13 +415,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>6</v>
@@ -432,13 +432,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s" s="0">
         <v>6</v>
@@ -446,50 +446,50 @@
     </row>
     <row r="17">
       <c r="B17" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>10</v>
@@ -497,19 +497,19 @@
     </row>
     <row r="20">
       <c r="B20" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -517,16 +517,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s" s="0">
         <v>6</v>
@@ -611,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s" s="0">
         <v>6</v>
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s" s="0">
         <v>6</v>
@@ -636,16 +636,16 @@
     </row>
     <row r="29">
       <c r="B29" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s" s="0">
         <v>6</v>
@@ -653,36 +653,36 @@
     </row>
     <row r="30">
       <c r="B30" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -690,16 +690,16 @@
         <v>6</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F32" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
@@ -707,16 +707,16 @@
         <v>6</v>
       </c>
       <c r="C33" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s" s="0">
         <v>7</v>
-      </c>
-      <c r="D33" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="F33" t="s" s="0">
-        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -724,16 +724,16 @@
         <v>6</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s" s="0">
         <v>6</v>
@@ -795,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E39" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>6</v>
@@ -812,13 +812,13 @@
         <v>6</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s" s="0">
         <v>6</v>
@@ -826,70 +826,70 @@
     </row>
     <row r="41">
       <c r="B41" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F43" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F44" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
@@ -897,16 +897,16 @@
         <v>6</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="E45" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="F45" t="s" s="0">
-        <v>12</v>
       </c>
     </row>
     <row r="46">
@@ -914,7 +914,7 @@
         <v>6</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s" s="0">
         <v>6</v>
@@ -982,16 +982,16 @@
     </row>
     <row r="51">
       <c r="B51" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F51" t="s" s="0">
         <v>6</v>
@@ -999,53 +999,53 @@
     </row>
     <row r="52">
       <c r="B52" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E54" t="s" s="0">
         <v>12</v>
       </c>
       <c r="F54" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
@@ -1056,10 +1056,10 @@
         <v>6</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E55" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F55" t="s" s="0">
         <v>14</v>
@@ -1073,13 +1073,13 @@
         <v>6</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57">
@@ -1178,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E63" t="s" s="0">
         <v>8</v>
@@ -1189,70 +1189,70 @@
     </row>
     <row r="64">
       <c r="B64" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F64" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E65" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F65" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E66" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F66" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E67" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68">
@@ -1260,16 +1260,16 @@
         <v>6</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E68" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69">
@@ -1277,16 +1277,16 @@
         <v>6</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F69" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70">
@@ -1294,7 +1294,7 @@
         <v>6</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s" s="0">
         <v>6</v>
@@ -1362,16 +1362,16 @@
     </row>
     <row r="75">
       <c r="B75" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E75" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s" s="0">
         <v>6</v>
@@ -1379,53 +1379,53 @@
     </row>
     <row r="76">
       <c r="B76" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D76" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E76" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F76" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D77" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E77" t="s" s="0">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E78" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
@@ -1436,13 +1436,13 @@
         <v>6</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E79" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F79" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
@@ -1453,13 +1453,13 @@
         <v>6</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E80" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F80" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
@@ -1558,10 +1558,10 @@
         <v>6</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E87" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F87" t="s" s="0">
         <v>6</v>
@@ -1569,67 +1569,67 @@
     </row>
     <row r="88">
       <c r="B88" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D88" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E88" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F88" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E89" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F89" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E90" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F90" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D91" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E91" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F91" t="s" s="0">
         <v>10</v>
@@ -1646,10 +1646,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F92" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93">
@@ -1657,16 +1657,16 @@
         <v>6</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E93" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F93" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94">
@@ -1674,7 +1674,7 @@
         <v>6</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D94" t="s" s="0">
         <v>6</v>
@@ -1742,16 +1742,16 @@
     </row>
     <row r="99">
       <c r="B99" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E99" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F99" t="s" s="0">
         <v>6</v>
@@ -1759,36 +1759,36 @@
     </row>
     <row r="100">
       <c r="B100" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E100" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F100" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D101" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E101" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F101" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102">
@@ -1796,16 +1796,16 @@
         <v>6</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D102" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E102" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F102" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103">
@@ -1813,16 +1813,16 @@
         <v>6</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D103" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E103" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F103" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104">
@@ -1830,16 +1830,16 @@
         <v>6</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D104" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E104" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F104" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105">
@@ -1847,7 +1847,7 @@
         <v>6</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D105" t="s" s="0">
         <v>6</v>
@@ -1932,53 +1932,53 @@
     </row>
     <row r="111">
       <c r="B111" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D111" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E111" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F111" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D112" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E112" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F112" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D113" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E113" t="s" s="0">
         <v>13</v>
       </c>
       <c r="F113" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114">
@@ -1986,13 +1986,13 @@
         <v>6</v>
       </c>
       <c r="C114" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D114" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E114" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F114" t="s" s="0">
         <v>7</v>
@@ -2003,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D115" t="s" s="0">
         <v>6</v>
@@ -2012,7 +2012,7 @@
         <v>6</v>
       </c>
       <c r="F115" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116">
@@ -2020,7 +2020,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D116" t="s" s="0">
         <v>6</v>
@@ -2122,16 +2122,16 @@
     </row>
     <row r="123">
       <c r="B123" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D123" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E123" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F123" t="s" s="0">
         <v>6</v>
@@ -2139,36 +2139,36 @@
     </row>
     <row r="124">
       <c r="B124" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D124" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E124" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F124" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D125" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E125" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F125" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126">
@@ -2176,16 +2176,16 @@
         <v>6</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D126" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E126" t="s" s="0">
         <v>13</v>
       </c>
       <c r="F126" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127">
@@ -2193,16 +2193,16 @@
         <v>6</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D127" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E127" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F127" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128">
@@ -2210,16 +2210,16 @@
         <v>6</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D128" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E128" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F128" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129">
@@ -2227,7 +2227,7 @@
         <v>6</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D129" t="s" s="0">
         <v>6</v>
@@ -2312,53 +2312,53 @@
     </row>
     <row r="135">
       <c r="B135" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C135" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D135" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E135" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F135" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C136" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E136" t="s" s="0">
         <v>13</v>
       </c>
       <c r="F136" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E137" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F137" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138">
@@ -2366,16 +2366,16 @@
         <v>6</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E138" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F138" t="s" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139">
@@ -2383,7 +2383,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D139" t="s" s="0">
         <v>6</v>
@@ -2392,7 +2392,7 @@
         <v>6</v>
       </c>
       <c r="F139" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140">
@@ -2400,7 +2400,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D140" t="s" s="0">
         <v>6</v>
@@ -2525,112 +2525,112 @@
         <v>6</v>
       </c>
       <c r="D148" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E148" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F148" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C149" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D149" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E149" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F149" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C150" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D150" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E150" t="s" s="0">
         <v>8</v>
       </c>
       <c r="F150" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C151" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D151" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E151" t="s" s="0">
         <v>12</v>
       </c>
       <c r="F151" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C152" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D152" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E152" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F152" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D153" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E153" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F153" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D154" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E154" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F154" t="s" s="0">
         <v>6</v>
@@ -2644,10 +2644,10 @@
         <v>6</v>
       </c>
       <c r="D155" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E155" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F155" t="s" s="0">
         <v>6</v>
@@ -2704,7 +2704,7 @@
         <v>6</v>
       </c>
       <c r="F159" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160">
@@ -2715,13 +2715,13 @@
         <v>6</v>
       </c>
       <c r="D160" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E160" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F160" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161">
@@ -2732,13 +2732,13 @@
         <v>6</v>
       </c>
       <c r="D161" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E161" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F161" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162">
@@ -2752,27 +2752,27 @@
         <v>9</v>
       </c>
       <c r="E162" t="s" s="0">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F162" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C163" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D163" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E163" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F163" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164">
@@ -2780,47 +2780,47 @@
         <v>8</v>
       </c>
       <c r="C164" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D164" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E164" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F164" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165">
       <c r="B165" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C165" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D165" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E165" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F165" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D166" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E166" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F166" t="s" s="0">
         <v>6</v>
@@ -2828,16 +2828,16 @@
     </row>
     <row r="167">
       <c r="B167" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C167" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D167" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E167" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F167" t="s" s="0">
         <v>6</v>
@@ -2905,47 +2905,47 @@
         <v>6</v>
       </c>
       <c r="D172" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E172" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F172" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173">
       <c r="B173" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D173" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E173" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F173" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C174" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D174" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E174" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F174" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175">
@@ -2953,64 +2953,64 @@
         <v>8</v>
       </c>
       <c r="C175" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D175" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E175" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F175" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C176" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D176" t="s" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E176" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F176" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C177" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D177" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E177" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F177" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178">
       <c r="B178" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C178" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D178" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E178" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F178" t="s" s="0">
         <v>6</v>
@@ -3024,10 +3024,10 @@
         <v>6</v>
       </c>
       <c r="D179" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E179" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F179" t="s" s="0">
         <v>6</v>
@@ -3084,7 +3084,7 @@
         <v>6</v>
       </c>
       <c r="F183" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184">
@@ -3095,13 +3095,13 @@
         <v>6</v>
       </c>
       <c r="D184" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E184" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F184" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185">
@@ -3112,13 +3112,13 @@
         <v>6</v>
       </c>
       <c r="D185" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E185" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F185" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="186">
@@ -3129,78 +3129,78 @@
         <v>6</v>
       </c>
       <c r="D186" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E186" t="s" s="0">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F186" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187">
       <c r="B187" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C187" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D187" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E187" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F187" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="188">
       <c r="B188" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C188" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D188" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E188" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F188" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189">
       <c r="B189" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C189" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D189" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E189" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C189" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D189" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E189" t="s" s="0">
-        <v>6</v>
-      </c>
       <c r="F189" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="190">
       <c r="B190" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C190" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D190" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E190" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F190" t="s" s="0">
         <v>6</v>
@@ -3208,16 +3208,16 @@
     </row>
     <row r="191">
       <c r="B191" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C191" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D191" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E191" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F191" t="s" s="0">
         <v>6</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="195">
       <c r="B195" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C195" t="s" s="0">
         <v>6</v>
@@ -3279,16 +3279,16 @@
     </row>
     <row r="196">
       <c r="B196" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C196" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D196" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E196" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F196" t="s" s="0">
         <v>6</v>
@@ -3296,87 +3296,87 @@
     </row>
     <row r="197">
       <c r="B197" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C197" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D197" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E197" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F197" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198">
       <c r="B198" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C198" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D198" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E198" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F198" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="199">
       <c r="B199" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C199" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D199" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E199" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F199" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200">
       <c r="B200" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C200" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D200" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E200" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F200" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201">
       <c r="B201" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C201" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D201" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E201" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F201" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202">
@@ -3393,7 +3393,7 @@
         <v>6</v>
       </c>
       <c r="F202" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="203">
@@ -3410,7 +3410,7 @@
         <v>6</v>
       </c>
       <c r="F203" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="204">
@@ -3427,7 +3427,7 @@
         <v>6</v>
       </c>
       <c r="F204" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="206">
@@ -3489,13 +3489,13 @@
         <v>6</v>
       </c>
       <c r="C209" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D209" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E209" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F209" t="s" s="0">
         <v>6</v>
@@ -3503,33 +3503,33 @@
     </row>
     <row r="210">
       <c r="B210" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C210" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D210" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E210" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F210" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="211">
       <c r="B211" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C211" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D211" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E211" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F211" t="s" s="0">
         <v>8</v>
@@ -3537,53 +3537,53 @@
     </row>
     <row r="212">
       <c r="B212" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C212" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D212" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E212" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F212" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213">
       <c r="B213" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C213" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D213" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E213" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F213" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="214">
       <c r="B214" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C214" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D214" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E214" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F214" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215">
@@ -3594,13 +3594,13 @@
         <v>6</v>
       </c>
       <c r="D215" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E215" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F215" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="216">
@@ -3611,13 +3611,13 @@
         <v>6</v>
       </c>
       <c r="D216" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E216" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F216" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218">
@@ -3642,7 +3642,7 @@
     </row>
     <row r="219">
       <c r="B219" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C219" t="s" s="0">
         <v>6</v>
@@ -3659,16 +3659,16 @@
     </row>
     <row r="220">
       <c r="B220" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C220" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D220" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E220" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F220" t="s" s="0">
         <v>6</v>
@@ -3676,87 +3676,87 @@
     </row>
     <row r="221">
       <c r="B221" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C221" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D221" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E221" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F221" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222">
       <c r="B222" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C222" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D222" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E222" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F222" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="223">
       <c r="B223" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C223" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D223" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E223" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F223" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="224">
       <c r="B224" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C224" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D224" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E224" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F224" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="225">
       <c r="B225" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C225" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D225" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E225" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F225" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="226">
@@ -3773,7 +3773,7 @@
         <v>6</v>
       </c>
       <c r="F226" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="227">
@@ -3790,7 +3790,7 @@
         <v>6</v>
       </c>
       <c r="F227" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228">
@@ -3807,7 +3807,7 @@
         <v>6</v>
       </c>
       <c r="F228" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="230">
@@ -3869,13 +3869,13 @@
         <v>6</v>
       </c>
       <c r="C233" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D233" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E233" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F233" t="s" s="0">
         <v>6</v>
@@ -3883,19 +3883,19 @@
     </row>
     <row r="234">
       <c r="B234" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C234" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D234" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E234" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F234" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="235">
@@ -3903,33 +3903,33 @@
         <v>9</v>
       </c>
       <c r="C235" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D235" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E235" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F235" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236">
       <c r="B236" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C236" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D236" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E236" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F236" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="237">
@@ -3937,33 +3937,33 @@
         <v>13</v>
       </c>
       <c r="C237" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D237" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E237" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F237" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="238">
       <c r="B238" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C238" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D238" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E238" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F238" t="s" s="0">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="239">
@@ -3974,13 +3974,13 @@
         <v>6</v>
       </c>
       <c r="D239" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E239" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F239" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="240">
@@ -3991,13 +3991,13 @@
         <v>6</v>
       </c>
       <c r="D240" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E240" t="s" s="0">
         <v>6</v>
       </c>
       <c r="F240" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="242">
@@ -4025,10 +4025,10 @@
         <v>6</v>
       </c>
       <c r="C243" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D243" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E243" t="s" s="0">
         <v>6</v>
@@ -4039,16 +4039,16 @@
     </row>
     <row r="244">
       <c r="B244" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C244" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D244" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E244" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F244" t="s" s="0">
         <v>6</v>
@@ -4056,92 +4056,92 @@
     </row>
     <row r="245">
       <c r="B245" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C245" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D245" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E245" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F245" t="s" s="0">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="246">
       <c r="B246" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C246" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D246" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E246" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F246" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="247">
       <c r="B247" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C247" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D247" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E247" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F247" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="248">
       <c r="B248" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C248" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D248" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E248" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F248" t="s" s="0">
         <v>7</v>
-      </c>
-      <c r="C248" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D248" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E248" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="F248" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="249">
       <c r="B249" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C249" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D249" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E249" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F249" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="250">
       <c r="B250" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C250" t="s" s="0">
         <v>6</v>
@@ -4153,7 +4153,7 @@
         <v>6</v>
       </c>
       <c r="F250" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251">
@@ -4229,109 +4229,109 @@
     </row>
     <row r="256">
       <c r="B256" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C256" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D256" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E256" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F256" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257">
       <c r="B257" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C257" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D257" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E257" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F257" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="258">
       <c r="B258" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C258" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D258" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E258" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F258" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259">
       <c r="B259" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C259" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D259" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E259" t="s" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F259" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260">
       <c r="B260" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C260" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D260" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E260" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F260" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="261">
       <c r="B261" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C261" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D261" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E261" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F261" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="262">
       <c r="B262" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C262" t="s" s="0">
         <v>6</v>
@@ -4340,15 +4340,15 @@
         <v>6</v>
       </c>
       <c r="E262" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F262" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="263">
       <c r="B263" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C263" t="s" s="0">
         <v>6</v>
@@ -4405,10 +4405,10 @@
         <v>6</v>
       </c>
       <c r="C267" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D267" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E267" t="s" s="0">
         <v>6</v>
@@ -4419,16 +4419,16 @@
     </row>
     <row r="268">
       <c r="B268" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C268" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D268" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E268" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F268" t="s" s="0">
         <v>6</v>
@@ -4436,50 +4436,50 @@
     </row>
     <row r="269">
       <c r="B269" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C269" t="s" s="0">
         <v>10</v>
       </c>
       <c r="D269" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E269" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F269" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="270">
       <c r="B270" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C270" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D270" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E270" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F270" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="271">
       <c r="B271" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C271" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D271" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E271" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F271" t="s" s="0">
         <v>13</v>
@@ -4490,38 +4490,38 @@
         <v>8</v>
       </c>
       <c r="C272" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D272" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E272" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F272" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="273">
       <c r="B273" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C273" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D273" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E273" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F273" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="274">
       <c r="B274" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C274" t="s" s="0">
         <v>6</v>
@@ -4533,7 +4533,7 @@
         <v>6</v>
       </c>
       <c r="F274" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="275">
@@ -4609,50 +4609,50 @@
     </row>
     <row r="280">
       <c r="B280" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C280" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D280" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E280" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F280" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="281">
       <c r="B281" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C281" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D281" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E281" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F281" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282">
       <c r="B282" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C282" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D282" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E282" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F282" t="s" s="0">
         <v>8</v>
@@ -4660,13 +4660,13 @@
     </row>
     <row r="283">
       <c r="B283" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C283" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D283" t="s" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E283" t="s" s="0">
         <v>7</v>
@@ -4677,19 +4677,19 @@
     </row>
     <row r="284">
       <c r="B284" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C284" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D284" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E284" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F284" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="285">
@@ -4697,21 +4697,21 @@
         <v>8</v>
       </c>
       <c r="C285" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D285" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E285" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F285" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="286">
       <c r="B286" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C286" t="s" s="0">
         <v>6</v>
@@ -4720,15 +4720,15 @@
         <v>6</v>
       </c>
       <c r="E286" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F286" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="287">
       <c r="B287" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C287" t="s" s="0">
         <v>6</v>
@@ -4785,13 +4785,13 @@
         <v>6</v>
       </c>
       <c r="C291" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D291" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E291" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F291" t="s" s="0">
         <v>6</v>
@@ -4802,13 +4802,13 @@
         <v>6</v>
       </c>
       <c r="C292" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D292" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E292" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F292" t="s" s="0">
         <v>6</v>
@@ -4819,13 +4819,13 @@
         <v>6</v>
       </c>
       <c r="C293" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D293" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E293" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F293" t="s" s="0">
         <v>6</v>
@@ -4839,13 +4839,13 @@
         <v>10</v>
       </c>
       <c r="D294" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E294" t="s" s="0">
         <v>8</v>
       </c>
       <c r="F294" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="295">
@@ -4853,30 +4853,30 @@
         <v>6</v>
       </c>
       <c r="C295" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D295" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E295" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F295" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="296">
       <c r="B296" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C296" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D296" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E296" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F296" t="s" s="0">
         <v>8</v>
@@ -4884,41 +4884,41 @@
     </row>
     <row r="297">
       <c r="B297" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C297" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D297" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E297" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F297" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="298">
       <c r="B298" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C298" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D298" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E298" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F298" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="299">
       <c r="B299" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C299" t="s" s="0">
         <v>6</v>
@@ -4927,15 +4927,15 @@
         <v>6</v>
       </c>
       <c r="E299" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F299" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="300">
       <c r="B300" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C300" t="s" s="0">
         <v>6</v>
@@ -4972,7 +4972,7 @@
     </row>
     <row r="303">
       <c r="B303" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C303" t="s" s="0">
         <v>6</v>
@@ -4989,16 +4989,16 @@
     </row>
     <row r="304">
       <c r="B304" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C304" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D304" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E304" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F304" t="s" s="0">
         <v>6</v>
@@ -5006,47 +5006,47 @@
     </row>
     <row r="305">
       <c r="B305" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C305" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D305" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E305" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C305" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D305" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="E305" t="s" s="0">
-        <v>11</v>
-      </c>
       <c r="F305" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="306">
       <c r="B306" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C306" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D306" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E306" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F306" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="307">
       <c r="B307" t="s" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C307" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D307" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E307" t="s" s="0">
         <v>8</v>
@@ -5057,19 +5057,19 @@
     </row>
     <row r="308">
       <c r="B308" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C308" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D308" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E308" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F308" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="309">
@@ -5080,10 +5080,10 @@
         <v>6</v>
       </c>
       <c r="D309" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E309" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F309" t="s" s="0">
         <v>13</v>
@@ -5097,13 +5097,13 @@
         <v>6</v>
       </c>
       <c r="D310" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E310" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F310" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="311">
@@ -5165,13 +5165,13 @@
         <v>6</v>
       </c>
       <c r="C315" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D315" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E315" t="s" s="0">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F315" t="s" s="0">
         <v>6</v>
@@ -5182,13 +5182,13 @@
         <v>6</v>
       </c>
       <c r="C316" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D316" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E316" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F316" t="s" s="0">
         <v>6</v>
@@ -5199,13 +5199,13 @@
         <v>6</v>
       </c>
       <c r="C317" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D317" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E317" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F317" t="s" s="0">
         <v>6</v>
@@ -5216,16 +5216,16 @@
         <v>6</v>
       </c>
       <c r="C318" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D318" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E318" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F318" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="319">
@@ -5233,72 +5233,72 @@
         <v>6</v>
       </c>
       <c r="C319" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D319" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E319" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F319" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="320">
       <c r="B320" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C320" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D320" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E320" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F320" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="321">
       <c r="B321" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C321" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D321" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E321" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F321" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="322">
       <c r="B322" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C322" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D322" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E322" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F322" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="323">
       <c r="B323" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C323" t="s" s="0">
         <v>6</v>
@@ -5307,15 +5307,15 @@
         <v>6</v>
       </c>
       <c r="E323" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F323" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="324">
       <c r="B324" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C324" t="s" s="0">
         <v>6</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="327">
       <c r="B327" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C327" t="s" s="0">
         <v>6</v>
@@ -5369,16 +5369,16 @@
     </row>
     <row r="328">
       <c r="B328" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C328" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D328" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E328" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F328" t="s" s="0">
         <v>6</v>
@@ -5386,36 +5386,36 @@
     </row>
     <row r="329">
       <c r="B329" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C329" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D329" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E329" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F329" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="330">
       <c r="B330" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C330" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D330" t="s" s="0">
         <v>11</v>
       </c>
       <c r="E330" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F330" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="331">
@@ -5423,21 +5423,21 @@
         <v>7</v>
       </c>
       <c r="C331" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D331" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E331" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F331" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="332">
       <c r="B332" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C332" t="s" s="0">
         <v>8</v>
@@ -5449,7 +5449,7 @@
         <v>8</v>
       </c>
       <c r="F332" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="333">
@@ -5460,13 +5460,13 @@
         <v>6</v>
       </c>
       <c r="D333" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E333" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F333" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="334">
@@ -5477,13 +5477,13 @@
         <v>6</v>
       </c>
       <c r="D334" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E334" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F334" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="335">
@@ -5548,69 +5548,69 @@
         <v>6</v>
       </c>
       <c r="D339" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E339" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F339" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="340">
       <c r="B340" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C340" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D340" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E340" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F340" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="341">
       <c r="B341" t="s" s="0">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C341" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D341" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E341" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F341" t="s" s="0">
         <v>7</v>
-      </c>
-      <c r="E341" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F341" t="s" s="0">
-        <v>11</v>
       </c>
     </row>
     <row r="342">
       <c r="B342" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C342" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D342" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E342" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F342" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="343">
       <c r="B343" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C343" t="s" s="0">
         <v>8</v>
@@ -5622,7 +5622,7 @@
         <v>8</v>
       </c>
       <c r="F343" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="344">
@@ -5630,16 +5630,16 @@
         <v>8</v>
       </c>
       <c r="C344" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D344" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E344" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F344" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="345">
@@ -5732,16 +5732,16 @@
     </row>
     <row r="351">
       <c r="B351" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C351" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D351" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E351" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F351" t="s" s="0">
         <v>6</v>
@@ -5749,16 +5749,16 @@
     </row>
     <row r="352">
       <c r="B352" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C352" t="s" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D352" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E352" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F352" t="s" s="0">
         <v>6</v>
@@ -5766,70 +5766,70 @@
     </row>
     <row r="353">
       <c r="B353" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C353" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D353" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E353" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F353" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="354">
       <c r="B354" t="s" s="0">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C354" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D354" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E354" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F354" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="355">
       <c r="B355" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C355" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D355" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E355" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F355" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="356">
       <c r="B356" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C356" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D356" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E356" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F356" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="357">
@@ -5846,7 +5846,7 @@
         <v>6</v>
       </c>
       <c r="F357" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="358">
@@ -5928,13 +5928,13 @@
         <v>6</v>
       </c>
       <c r="D363" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E363" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F363" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="364">
@@ -5942,84 +5942,84 @@
         <v>10</v>
       </c>
       <c r="C364" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D364" t="s" s="0">
         <v>11</v>
       </c>
       <c r="E364" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F364" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="365">
       <c r="B365" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C365" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D365" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E365" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F365" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="366">
       <c r="B366" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C366" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D366" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E366" t="s" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F366" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="367">
       <c r="B367" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C367" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D367" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E367" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F367" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="368">
       <c r="B368" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C368" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D368" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E368" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F368" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="369">
@@ -6112,16 +6112,16 @@
     </row>
     <row r="375">
       <c r="B375" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C375" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D375" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E375" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F375" t="s" s="0">
         <v>6</v>
@@ -6129,16 +6129,16 @@
     </row>
     <row r="376">
       <c r="B376" t="s" s="0">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C376" t="s" s="0">
         <v>12</v>
       </c>
       <c r="D376" t="s" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E376" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F376" t="s" s="0">
         <v>6</v>
@@ -6149,16 +6149,16 @@
         <v>8</v>
       </c>
       <c r="C377" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D377" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E377" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F377" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="378">
@@ -6166,50 +6166,50 @@
         <v>7</v>
       </c>
       <c r="C378" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D378" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E378" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F378" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="379">
       <c r="B379" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C379" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D379" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E379" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F379" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="380">
       <c r="B380" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C380" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D380" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E380" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F380" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="381">
@@ -6226,7 +6226,7 @@
         <v>6</v>
       </c>
       <c r="F381" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="382">

</xml_diff>